<commit_message>
1. Single user- Submission & Forward and then Submission 2. Multi user- Submission & Forward and then Submission
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Transmittals_New" sheetId="1" r:id="rId1"/>
+    <sheet name="Transmittals_New_ActionRequired" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
   <si>
     <t>To</t>
   </si>
@@ -66,9 +67,6 @@
     <t>Issued for Review</t>
   </si>
   <si>
-    <t>Comments for Issued for Review</t>
-  </si>
-  <si>
     <t>AttachDocuments</t>
   </si>
   <si>
@@ -100,6 +98,15 @@
   </si>
   <si>
     <t>AutoTestAdmin@@AutoTestUser</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>SPInstall</t>
+  </si>
+  <si>
+    <t>Submission</t>
   </si>
 </sst>
 </file>
@@ -500,7 +507,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -542,19 +764,19 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -571,10 +793,10 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -589,48 +811,25 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
       <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data for ReplyAll and Delegate
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="33">
   <si>
     <t>To</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>Submission</t>
+  </si>
+  <si>
+    <t>DelegateTo</t>
+  </si>
+  <si>
+    <t>Delegate- Message for New transmittal</t>
+  </si>
+  <si>
+    <t>Delegate</t>
+  </si>
+  <si>
+    <t>Reply All- Message for New transmittal</t>
+  </si>
+  <si>
+    <t>ReplyAll</t>
   </si>
 </sst>
 </file>
@@ -504,9 +519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -526,7 +543,7 @@
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,10 +587,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -614,7 +634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -640,7 +660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -677,11 +697,11 @@
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -706,11 +726,11 @@
       <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -748,7 +768,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -768,6 +788,64 @@
         <v>5</v>
       </c>
       <c r="M7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Included OverDue test data.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForReview.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_S5_NR\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Transmittals_New" sheetId="1" r:id="rId1"/>
     <sheet name="Transmittals_New_ActionRequired" sheetId="2" r:id="rId2"/>
+    <sheet name="Transmittals_Overdue" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="48">
   <si>
     <t>To</t>
   </si>
@@ -155,6 +156,15 @@
   </si>
   <si>
     <t>Mess</t>
+  </si>
+  <si>
+    <t>Message for New transmittal -Overdue</t>
+  </si>
+  <si>
+    <t>Overdue</t>
+  </si>
+  <si>
+    <t>LATFLD-00</t>
   </si>
 </sst>
 </file>
@@ -566,9 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -1023,7 +1031,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -1151,4 +1161,115 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>